<commit_message>
fully correct law dates (ahead version)
</commit_message>
<xml_diff>
--- a/Data/auxiliary_data.xlsx
+++ b/Data/auxiliary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9adb48ff0228f9c1/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="805" documentId="11_F25DC773A252ABDACC10483D791960605BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65329856-5EB6-4F2F-81AF-5296EFF334AE}"/>
+  <xr:revisionPtr revIDLastSave="813" documentId="11_F25DC773A252ABDACC10483D791960605BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0177690-0B5C-4A93-8549-7E8E333A705F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,7 +621,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -1672,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="5">
-        <v>0</v>
+        <v>2019</v>
       </c>
       <c r="D26" s="2">
-        <v>0</v>
+        <v>201810</v>
       </c>
       <c r="E26" s="5">
         <v>2020</v>
@@ -2325,13 +2325,13 @@
         <v>39</v>
       </c>
       <c r="B42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="5">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D42" s="2">
-        <v>201807</v>
+        <v>201805</v>
       </c>
       <c r="E42" s="5">
         <v>2018</v>
@@ -2697,10 +2697,10 @@
         <v>1</v>
       </c>
       <c r="C51" s="5">
-        <v>2017</v>
+        <v>0</v>
       </c>
       <c r="D51" s="2">
-        <v>201704</v>
+        <v>0</v>
       </c>
       <c r="E51" s="5">
         <v>0</v>

</xml_diff>